<commit_message>
lab report work, image_analyser.py worked on - cleaned up the methods section - worked a tiny bit more with results - finished off chi-squared calculator, stupidly big values but oh well - add images into the lab report for chi-squared?
</commit_message>
<xml_diff>
--- a/lab_reports/optical_fourier_transforms/results/Finding-x.xlsx
+++ b/lab_reports/optical_fourier_transforms/results/Finding-x.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="not sure what this was" sheetId="1" r:id="rId1"/>
-    <sheet name="actual sheet" sheetId="2" r:id="rId2"/>
+    <sheet name="nicer formatting" sheetId="3" r:id="rId2"/>
+    <sheet name="actual sheet" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>F Spacing (Pixels)</t>
   </si>
@@ -106,6 +107,21 @@
   </si>
   <si>
     <t>never recored</t>
+  </si>
+  <si>
+    <t>Nicer formatting</t>
+  </si>
+  <si>
+    <t>error (pixels)</t>
+  </si>
+  <si>
+    <t>Real Spacing (mm)</t>
+  </si>
+  <si>
+    <t>error (mm)</t>
+  </si>
+  <si>
+    <t>Fourier Spacing, u (pixels)</t>
   </si>
 </sst>
 </file>
@@ -165,12 +181,87 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -179,13 +270,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -661,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -970,10 +1076,108 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="C5:G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <f>(4723.79-427.722)/17</f>
+        <v>252.70988235294118</v>
+      </c>
+      <c r="E6" s="8">
+        <v>22</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0.10713692020238</v>
+      </c>
+      <c r="G6" s="10">
+        <v>2.6466459016870839E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="6">
+        <v>2</v>
+      </c>
+      <c r="D7" s="7">
+        <f>(5025.47-102.823)/20</f>
+        <v>246.13235</v>
+      </c>
+      <c r="E7" s="8">
+        <v>17</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.11</v>
+      </c>
+      <c r="G7" s="12">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="13">
+        <v>3</v>
+      </c>
+      <c r="D8" s="14">
+        <f>(6026.21-70.5645)/11</f>
+        <v>541.42231818181813</v>
+      </c>
+      <c r="E8" s="15">
+        <v>28</v>
+      </c>
+      <c r="F8" s="16">
+        <v>5.0006358420762287E-2</v>
+      </c>
+      <c r="G8" s="17">
+        <v>1.0586009005001187E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="K6" sqref="K6:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
work has been done, first draft of lab report done - diagrams have been changed about, the formatting of them - worked on discussion - completed the abstract - completed the conclusion - completed the appendix - first draft of this report is finished
</commit_message>
<xml_diff>
--- a/lab_reports/optical_fourier_transforms/results/Finding-x.xlsx
+++ b/lab_reports/optical_fourier_transforms/results/Finding-x.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\level_1\Level 2\RLI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackycao/Documents/Projects/degree_level2/lab_reports/optical_fourier_transforms/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="14680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="not sure what this was" sheetId="1" r:id="rId1"/>
     <sheet name="nicer formatting" sheetId="3" r:id="rId2"/>
     <sheet name="actual sheet" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>F Spacing (Pixels)</t>
   </si>
@@ -70,21 +76,6 @@
     <t>F Spacing, u (pixels)</t>
   </si>
   <si>
-    <t xml:space="preserve">error </t>
-  </si>
-  <si>
-    <t>error</t>
-  </si>
-  <si>
-    <t>relative error</t>
-  </si>
-  <si>
-    <t>pixel size F (m)</t>
-  </si>
-  <si>
-    <t>error (m)</t>
-  </si>
-  <si>
     <t>error(mm)</t>
   </si>
   <si>
@@ -122,13 +113,37 @@
   </si>
   <si>
     <t>Fourier Spacing, u (pixels)</t>
+  </si>
+  <si>
+    <t>relative error (alpha_R(P))</t>
+  </si>
+  <si>
+    <t>error (alpha_u)</t>
+  </si>
+  <si>
+    <t>relative error (alpha_R(u))</t>
+  </si>
+  <si>
+    <t>error (alpha_(u^-1))</t>
+  </si>
+  <si>
+    <t>relative error (alpha_[R(P)+R(u)])</t>
+  </si>
+  <si>
+    <t>error (m) (alpha_x)</t>
+  </si>
+  <si>
+    <t>error (alpha_P)</t>
+  </si>
+  <si>
+    <t>pixel size F (m), P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +161,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,16 +222,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -208,16 +239,16 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -227,7 +258,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -235,12 +266,12 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -249,26 +280,28 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -293,9 +326,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -331,7 +366,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18F45EDE-2F68-4CB0-B7EF-36B8E85F8869}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{18F45EDE-2F68-4CB0-B7EF-36B8E85F8869}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -406,7 +441,7 @@
         <xdr:cNvPr id="3" name="TextBox 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4F7BF8A-3424-4DE5-BDCA-A8C74F8CB819}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D4F7BF8A-3424-4DE5-BDCA-A8C74F8CB819}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -771,16 +806,16 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>7</v>
       </c>
@@ -794,7 +829,7 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -817,7 +852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -845,7 +880,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -874,7 +909,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -902,7 +937,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C8">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -921,7 +956,7 @@
       </c>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C9">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -939,7 +974,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -957,7 +992,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -975,7 +1010,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -993,7 +1028,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C13">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1011,7 +1046,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C14">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1029,7 +1064,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C15">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1047,7 +1082,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D16" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
@@ -1057,13 +1092,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G17" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G18" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -1078,42 +1113,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="C5:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C5" s="18" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C6" s="6">
         <v>1</v>
       </c>
@@ -1131,7 +1166,7 @@
         <v>2.6466459016870839E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C7" s="6">
         <v>2</v>
       </c>
@@ -1149,7 +1184,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C8" s="13">
         <v>3</v>
       </c>
@@ -1176,40 +1211,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:L8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="55" zoomScalePageLayoutView="55" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.7109375" customWidth="1"/>
-    <col min="8" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1640625" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" customWidth="1"/>
-    <col min="17" max="17" width="23.28515625" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
+    <col min="17" max="17" width="23.33203125" customWidth="1"/>
+    <col min="18" max="18" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H2">
         <f>E7/B7</f>
         <v>36.935043649926918</v>
@@ -1223,7 +1260,7 @@
         <v>0.15997762253445424</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1231,49 +1268,49 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="K5" t="s">
         <v>12</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="M5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="N5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="O5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="P5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1330,7 +1367,7 @@
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1389,7 +1426,7 @@
         <v>0.12479999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1451,23 +1488,24 @@
         <v>0.127</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="K12" s="4"/>
       <c r="L12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="O12" s="5"/>
       <c r="P12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="L13" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>